<commit_message>
MàJ méd gé + pharma
</commit_message>
<xml_diff>
--- a/dumas/dumas_specialite.xlsx
+++ b/dumas/dumas_specialite.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="101">
   <si>
     <t>DUMAS</t>
   </si>
@@ -231,9 +231,6 @@
     <t xml:space="preserve">  * choisissant la spécialité avec le menu déroulant en `C5` (cliquez sur la flèche en bas à droite de la cellule ou appuyer sur `Alt + flèche du bas`) ;</t>
   </si>
   <si>
-    <t>Choisir le domaine</t>
-  </si>
-  <si>
     <t>Spécialités (Médecine spécialisée)</t>
   </si>
   <si>
@@ -273,13 +270,58 @@
     <t>Code Pharma</t>
   </si>
   <si>
-    <t>???</t>
-  </si>
-  <si>
     <t>Méd spé</t>
   </si>
   <si>
     <t>Pharma</t>
+  </si>
+  <si>
+    <t>Officine</t>
+  </si>
+  <si>
+    <t>Pharmacie hospitalière bio-médicale</t>
+  </si>
+  <si>
+    <t>Industrie Recherche</t>
+  </si>
+  <si>
+    <t>Toxicologie</t>
+  </si>
+  <si>
+    <t>Industrie</t>
+  </si>
+  <si>
+    <t>788</t>
+  </si>
+  <si>
+    <t>790</t>
+  </si>
+  <si>
+    <t>844</t>
+  </si>
+  <si>
+    <t>Sciences Pharmaceutiques</t>
+  </si>
+  <si>
+    <t>Biologie médicale</t>
+  </si>
+  <si>
+    <t>159</t>
+  </si>
+  <si>
+    <t>Pharmacie hospitalière et des collectivités</t>
+  </si>
+  <si>
+    <t>Pharmacie hospitalière - Pratique et recherche</t>
+  </si>
+  <si>
+    <t>Pharmacie hospitalière - Pharmacie industrielle et biologie médicale</t>
+  </si>
+  <si>
+    <t>Innovation pharmaceutique et recherche</t>
+  </si>
+  <si>
+    <t>Choisir le domaine ↓</t>
   </si>
 </sst>
 </file>
@@ -391,11 +433,13 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right/>
+      <top style="thin">
         <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -737,7 +781,7 @@
   <dimension ref="A1:G71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -745,6 +789,7 @@
     <col min="1" max="1" width="109" customWidth="1"/>
     <col min="3" max="3" width="44.42578125" customWidth="1"/>
     <col min="4" max="4" width="36.28515625" customWidth="1"/>
+    <col min="6" max="6" width="33" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="51" x14ac:dyDescent="0.75">
@@ -757,12 +802,12 @@
         <v>1</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>70</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C3" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="32.25" x14ac:dyDescent="0.5">
@@ -778,15 +823,15 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>20</v>
       </c>
       <c r="D5" s="12" t="str">
-        <f ca="1">C27 &amp; VLOOKUP(C3,domaines,2,FALSE) &amp; C28 &amp; C29&amp;
-IF(C3="Médecine spécialisée",C30&amp; VLOOKUP(C5,listSpe,2,FALSE),IF(C3="Pharmacie",C30&amp; VLOOKUP(C6,listSpePharma,2,FALSE),""))</f>
-        <v>document.getElementById("list_domain").innerHTML += '&lt;li style="display: block" class="margin-top-5"&gt;&lt;input type="hidden" value="sdv" name="domain[]"&gt;&lt;span class="label label-primary" style="font-size: inherit; display: inline-block; text-align: justify; white-space: normal; padding: 0px; height: 20px;" data-html="true" data-toggle="tooltip" data-original-title="&lt;span style=&amp;quot;display: block; text-align: left; padding-left: 0px&amp;quot;&gt;Sciences du Vivant [q-bio]&lt;/span&gt;"&gt;&lt;i style="border-radius: 0px; height: 20px; padding: 0px; margin: 0px 7px; top: 1px; bottom: 0px;" class="glyphicon glyphicon-move move" data-toggle="tooltip" data-original-title="Déplacer" data-placement="left"&gt;&lt;/i&gt;&lt;span style="padding-top: 4px; padding-bottom: 0px; margin-top: 0px; height: 20px; display: inline-block;"&gt;Sciences du Vivant [q-bio]&lt;/span&gt;&lt;button style="height: 20px; padding-top: 0px; padding-bottom: 0px; margin-left: 10px; margin-top: -2px; margin-right: 0px; border: medium none ! important; padding-right: 6px;" class="btn btn-xs btn-primary" type="button" data-toggle="tooltip" data-original-title="Supprimer" data-placement="right"&gt;&lt;i class="glyphicon glyphicon-trash"&gt;&lt;/i&gt;&lt;/button&gt;&lt;/span&gt;&lt;/li&gt;&lt;li style="display: block" class="margin-top-5"&gt;&lt;input type="hidden" value="sdv.mhep" name="domain[]"&gt;&lt;span class="label label-primary" style="font-size: inherit; display: inline-block; text-align: justify; white-space: normal; padding: 0px; height: 20px;" data-html="true" data-toggle="tooltip" data-original-title="&lt;span style=&amp;quot;display: block; text-align: left; padding-left: 0px&amp;quot;&gt;Sciences du Vivant [q-bio]&lt;/span&gt;&lt;span style=&amp;quot;display: block; text-align: left; padding-left: 15px&amp;quot;&gt;&lt;i class=&amp;quot;glyphicon glyphicon-share-alt&amp;quot; style=&amp;quot;transform: scaleY(-1);&amp;quot;&gt;&lt;/i&gt; Médecine humaine et pathologie&lt;/span&gt;"&gt;&lt;i style="border-radius: 0px; height: 20px; padding: 0px; margin: 0px 7px; top: 1px; bottom: 0px;" class="glyphicon glyphicon-move move" data-toggle="tooltip" data-original-title="Déplacer" data-placement="left"&gt;&lt;/i&gt;&lt;span style="padding-top: 4px; padding-bottom: 0px; margin-top: 0px; height: 20px; display: inline-block;"&gt;Médecine humaine et pathologie&lt;/span&gt;&lt;button style="height: 20px; padding-top: 0px; padding-bottom: 0px; margin-left: 10px; margin-top: -2px; margin-right: 0px; border: medium none ! important; padding-right: 6px;" class="btn btn-xs btn-primary" type="button" data-toggle="tooltip" data-original-title="Supprimer" data-placement="right"&gt;&lt;i class="glyphicon glyphicon-trash"&gt;&lt;/i&gt;&lt;/button&gt;&lt;/span&gt;&lt;/li&gt;';13document.getElementById("dumas_degreeType").value = ; document.getElementById("dumas_degreeSubject").value = 48; document.getElementById("dumas_degreeSpeciality").value = ???</v>
+        <f ca="1">C27 &amp; C28 &amp; VLOOKUP(C3,domaines,2,FALSE) &amp; C29&amp;
+IF(C3="Médecine spécialisée",C30&amp; VLOOKUP(C5,listSpe,2,FALSE),IF(C3="Pharmacie",C30&amp; VLOOKUP(C6,listSpePharma,2,FALSE),IF(C3="Médecine générale",C30&amp; "150","")))</f>
+        <v>document.getElementById("list_domain").innerHTML += '&lt;li style="display: block" class="margin-top-5"&gt;&lt;input type="hidden" value="sdv" name="domain[]"&gt;&lt;span class="label label-primary" style="font-size: inherit; display: inline-block; text-align: justify; white-space: normal; padding: 0px; height: 20px;" data-html="true" data-toggle="tooltip" data-original-title="&lt;span style=&amp;quot;display: block; text-align: left; padding-left: 0px&amp;quot;&gt;Sciences du Vivant [q-bio]&lt;/span&gt;"&gt;&lt;i style="border-radius: 0px; height: 20px; padding: 0px; margin: 0px 7px; top: 1px; bottom: 0px;" class="glyphicon glyphicon-move move" data-toggle="tooltip" data-original-title="Déplacer" data-placement="left"&gt;&lt;/i&gt;&lt;span style="padding-top: 4px; padding-bottom: 0px; margin-top: 0px; height: 20px; display: inline-block;"&gt;Sciences du Vivant [q-bio]&lt;/span&gt;&lt;button style="height: 20px; padding-top: 0px; padding-bottom: 0px; margin-left: 10px; margin-top: -2px; margin-right: 0px; border: medium none ! important; padding-right: 6px;" class="btn btn-xs btn-primary" type="button" data-toggle="tooltip" data-original-title="Supprimer" data-placement="right"&gt;&lt;i class="glyphicon glyphicon-trash"&gt;&lt;/i&gt;&lt;/button&gt;&lt;/span&gt;&lt;/li&gt;&lt;li style="display: block" class="margin-top-5"&gt;&lt;input type="hidden" value="sdv.mhep" name="domain[]"&gt;&lt;span class="label label-primary" style="font-size: inherit; display: inline-block; text-align: justify; white-space: normal; padding: 0px; height: 20px;" data-html="true" data-toggle="tooltip" data-original-title="&lt;span style=&amp;quot;display: block; text-align: left; padding-left: 0px&amp;quot;&gt;Sciences du Vivant [q-bio]&lt;/span&gt;&lt;span style=&amp;quot;display: block; text-align: left; padding-left: 15px&amp;quot;&gt;&lt;i class=&amp;quot;glyphicon glyphicon-share-alt&amp;quot; style=&amp;quot;transform: scaleY(-1);&amp;quot;&gt;&lt;/i&gt; Médecine humaine et pathologie&lt;/span&gt;"&gt;&lt;i style="border-radius: 0px; height: 20px; padding: 0px; margin: 0px 7px; top: 1px; bottom: 0px;" class="glyphicon glyphicon-move move" data-toggle="tooltip" data-original-title="Déplacer" data-placement="left"&gt;&lt;/i&gt;&lt;span style="padding-top: 4px; padding-bottom: 0px; margin-top: 0px; height: 20px; display: inline-block;"&gt;Médecine humaine et pathologie&lt;/span&gt;&lt;button style="height: 20px; padding-top: 0px; padding-bottom: 0px; margin-left: 10px; margin-top: -2px; margin-right: 0px; border: medium none ! important; padding-right: 6px;" class="btn btn-xs btn-primary" type="button" data-toggle="tooltip" data-original-title="Supprimer" data-placement="right"&gt;&lt;i class="glyphicon glyphicon-trash"&gt;&lt;/i&gt;&lt;/button&gt;&lt;/span&gt;&lt;/li&gt;';document.getElementById("dumas_degreeType").value = 13; document.getElementById("dumas_degreeSubject").value = 48; document.getElementById("dumas_degreeSpeciality").value = 159</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -794,10 +839,10 @@
         <v>2</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -888,7 +933,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>19</v>
@@ -897,16 +942,16 @@
         <v>67</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E26" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="F26" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="F26" s="7" t="s">
+      <c r="G26" s="7" t="s">
         <v>82</v>
-      </c>
-      <c r="G26" s="7" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -917,19 +962,19 @@
         <v>383</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="E27" s="8">
+        <v>76</v>
+      </c>
+      <c r="E27" s="13">
         <v>12</v>
       </c>
-      <c r="F27" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="G27" s="13" t="s">
-        <v>84</v>
+      <c r="F27" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -940,13 +985,19 @@
         <v>164</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="E28" s="8">
+        <v>77</v>
+      </c>
+      <c r="E28" s="13">
         <v>12</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -957,13 +1008,19 @@
         <v>196</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="E29" s="8">
+        <v>78</v>
+      </c>
+      <c r="E29" s="13">
         <v>13</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -974,13 +1031,19 @@
         <v>163</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="E30" s="8">
+        <v>79</v>
+      </c>
+      <c r="E30" s="13">
         <v>30</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="G30" s="8">
+        <v>592</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -990,6 +1053,12 @@
       <c r="B31" s="8">
         <v>159</v>
       </c>
+      <c r="F31" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
@@ -998,48 +1067,84 @@
       <c r="B32" s="8">
         <v>159</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F32" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="G32" s="8">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>26</v>
       </c>
       <c r="B33" s="8">
         <v>170</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F33" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="G33" s="8">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>27</v>
       </c>
       <c r="B34" s="8">
         <v>199</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F34" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="G34" s="8">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
         <v>28</v>
       </c>
       <c r="B35" s="8">
         <v>171</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F35" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="G35" s="8">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>29</v>
       </c>
       <c r="B36" s="8">
         <v>44</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F36" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G36" s="8">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
         <v>30</v>
       </c>
       <c r="B37" s="8">
         <v>206</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F37" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="G37" s="8">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
         <v>31</v>
       </c>
@@ -1047,7 +1152,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
         <v>32</v>
       </c>
@@ -1055,7 +1160,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
         <v>33</v>
       </c>
@@ -1063,7 +1168,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
         <v>34</v>
       </c>
@@ -1071,7 +1176,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
         <v>35</v>
       </c>
@@ -1079,7 +1184,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
         <v>36</v>
       </c>
@@ -1087,7 +1192,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
         <v>37</v>
       </c>
@@ -1095,7 +1200,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
         <v>38</v>
       </c>
@@ -1103,7 +1208,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
         <v>39</v>
       </c>
@@ -1111,7 +1216,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
         <v>40</v>
       </c>
@@ -1119,7 +1224,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
         <v>41</v>
       </c>
@@ -1312,6 +1417,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState ref="F27:G37">
+    <sortCondition ref="F27:F37"/>
+  </sortState>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5">
       <formula1>INDEX(listSpe,,1)</formula1>

</xml_diff>